<commit_message>
feat: udistrital/sga_cliente#1392 ajuste generador consolidado version pdf
- Se ajusta reporte generador consolidado para version pdf del mismo, tal acción involucró las siguientes mejoras
  - Tamaño custom de hoja pdf si se requiere, tamaño y espaciado de fuente, ajuste de texto en celdas que no están unidas, color en celdas que no tienen texto, fondo transparente cuando es blanco (250 para arriba en los canales rgb), distinción de fondo, cuadrícula, text, e imagenes por capas, indice de hojas, conteo de paginas pdf por cada sheet de excel (esto para encabezados personalizados)
  - Nota: **Se recomienda usar VALUE() en conciones de formula excel, esto para evitar fallos en el calculador de formulas de excelize**
</commit_message>
<xml_diff>
--- a/static/templates/Verif_Cump_PTD.xlsx
+++ b/static/templates/Verif_Cump_PTD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\go\src\github.com\udistrital\sga_mid\static\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{694464FD-225F-4FA7-AC04-9B8E4769C0DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E2AE8A-9886-49D0-AE78-5E214BEF0C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,17 +17,8 @@
     <sheet name="TCO" sheetId="2" r:id="rId2"/>
     <sheet name="MTO" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -38,29 +29,31 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>nefa</author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{612B361B-A091-4BC8-9DCA-C0B886F5CF36}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Desglose por proyectos curriculares para carga lectiva</t>
         </r>
       </text>
     </comment>
-    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{45330CCD-FFB0-4C71-9679-86EC7011BFCC}">
+    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: horas por proyecto
@@ -68,13 +61,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI4" authorId="0" shapeId="0" xr:uid="{A4610DEB-87CF-4D9A-B610-45D2A4915904}">
+    <comment ref="AI4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: # asignaturas por proyecto
@@ -82,13 +76,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK4" authorId="0" shapeId="0" xr:uid="{68F128BC-5FD7-4F05-B215-900955857CD3}">
+    <comment ref="AK4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: # grupos por proyecto
@@ -96,13 +91,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM4" authorId="0" shapeId="0" xr:uid="{131F946A-BF90-4739-A73F-1995AC63F1E2}">
+    <comment ref="AM4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Desglose de asignaturas por proyecto curricular</t>
@@ -116,29 +112,31 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>nefa</author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{263CB075-3E5F-4652-9353-226021702077}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Desglose por proyectos curriculares para carga lectiva</t>
         </r>
       </text>
     </comment>
-    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{36403384-CCE2-4F3A-A6CB-C7E404067D09}">
+    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: horas por proyecto
@@ -146,13 +144,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI4" authorId="0" shapeId="0" xr:uid="{9F3C0FA1-3C0A-4558-81F9-544A98714D87}">
+    <comment ref="AI4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: # asignaturas por proyecto
@@ -160,13 +159,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK4" authorId="0" shapeId="0" xr:uid="{C80CB719-5DF7-4C7F-9052-91B9AEF603E8}">
+    <comment ref="AK4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: # grupos por proyecto
@@ -174,13 +174,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM4" authorId="0" shapeId="0" xr:uid="{47ACFCB9-AB36-4124-8358-98BA9CB04AE1}">
+    <comment ref="AM4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Desglose de asignaturas por proyecto curricular</t>
@@ -194,29 +195,31 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>nefa</author>
+    <author/>
   </authors>
   <commentList>
-    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{E0822174-303C-41C0-8E6D-8CB0A1AED92D}">
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Desglose por proyectos curriculares para carga lectiva</t>
         </r>
       </text>
     </comment>
-    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{054AD0D6-5B76-4720-8C5A-5926246F7D05}">
+    <comment ref="AG4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: horas por proyecto
@@ -224,13 +227,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI4" authorId="0" shapeId="0" xr:uid="{2F7A243E-6A4F-4847-A7A6-9FFDB0523072}">
+    <comment ref="AI4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: # asignaturas por proyecto
@@ -238,13 +242,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK4" authorId="0" shapeId="0" xr:uid="{17C0EC1F-1C2E-4889-933F-7C79BC3285B5}">
+    <comment ref="AK4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Columna izquierda: # grupos por proyecto
@@ -252,13 +257,14 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM4" authorId="0" shapeId="0" xr:uid="{83817424-A508-4252-AC85-DEABE4B06251}">
+    <comment ref="AM4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
             <charset val="1"/>
           </rPr>
           <t>Desglose de asignaturas por proyecto curricular</t>
@@ -270,18 +276,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="59">
-  <si>
-    <t>udistrital img</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="57">
   <si>
     <t>FORMATO DE CONTROL DEL CUMPLIMIENTO DE LA NORMATIVA VIGENTE DEL PLAN DE TRABAJO DOCENTE</t>
   </si>
   <si>
     <t>Código: GD-PR-008-FR-004</t>
-  </si>
-  <si>
-    <t>sigud img</t>
   </si>
   <si>
     <t>Macroproceso: Gestión Académica</t>
@@ -462,7 +462,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -507,15 +507,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -533,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -627,39 +623,38 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -672,44 +667,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,9 +704,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1420920</xdr:colOff>
+      <xdr:colOff>1417320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>238320</xdr:rowOff>
+      <xdr:rowOff>234720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -762,7 +727,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="439200" y="30600"/>
-          <a:ext cx="981720" cy="826920"/>
+          <a:ext cx="978120" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -783,9 +748,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1132845</xdr:colOff>
+      <xdr:colOff>1129320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>208440</xdr:rowOff>
+      <xdr:rowOff>204840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -805,7 +770,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9701640" y="57240"/>
-          <a:ext cx="2303640" cy="770400"/>
+          <a:ext cx="2233440" cy="766800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -831,9 +796,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1420920</xdr:colOff>
+      <xdr:colOff>1417320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>238320</xdr:rowOff>
+      <xdr:rowOff>234720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -854,7 +819,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="439200" y="30600"/>
-          <a:ext cx="981720" cy="826920"/>
+          <a:ext cx="978120" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -875,9 +840,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1132845</xdr:colOff>
+      <xdr:colOff>1129320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>208440</xdr:rowOff>
+      <xdr:rowOff>204840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -897,7 +862,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9701640" y="57240"/>
-          <a:ext cx="2303640" cy="770400"/>
+          <a:ext cx="2233440" cy="766800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -923,9 +888,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1420920</xdr:colOff>
+      <xdr:colOff>1417320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>238320</xdr:rowOff>
+      <xdr:rowOff>234720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -946,7 +911,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="439200" y="30600"/>
-          <a:ext cx="981720" cy="826920"/>
+          <a:ext cx="978120" cy="823320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -967,9 +932,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>1132845</xdr:colOff>
+      <xdr:colOff>1129320</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>208440</xdr:rowOff>
+      <xdr:rowOff>204840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -989,7 +954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9701640" y="57240"/>
-          <a:ext cx="2303640" cy="770400"/>
+          <a:ext cx="2233440" cy="766800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1301,7 +1266,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AX5"/>
+  <dimension ref="A1:AX9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" ySplit="4" topLeftCell="E5" activePane="bottomRight" state="frozen"/>
@@ -1331,271 +1296,322 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="8"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="13"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:50" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="AD2" s="1"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="AD2" s="9"/>
     </row>
     <row r="3" spans="1:50" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="AD3" s="9"/>
+      <c r="AP3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="17" t="s">
+      <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AS3" s="3"/>
+      <c r="AT3" s="3"/>
+      <c r="AU3" s="3"/>
+      <c r="AV3" s="3"/>
+      <c r="AW3" s="3"/>
+      <c r="AX3" s="3"/>
+    </row>
+    <row r="4" spans="1:50" ht="102.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="AD3" s="1"/>
-      <c r="AP3" s="12" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="12"/>
-      <c r="AR3" s="12"/>
-      <c r="AS3" s="12"/>
-      <c r="AT3" s="12"/>
-      <c r="AU3" s="12"/>
-      <c r="AV3" s="12"/>
-      <c r="AW3" s="12"/>
-      <c r="AX3" s="12"/>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ4" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="AT4" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AU4" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AV4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AW4" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AX4" s="13" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="4" spans="1:50" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AS4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="AT4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU4" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AV4" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="AW4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AX4" s="4" t="s">
-        <v>55</v>
-      </c>
+    <row r="5" spans="1:50" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
+        <v>0</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0</v>
+      </c>
+      <c r="O5" s="15">
+        <v>0</v>
+      </c>
+      <c r="P5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>0</v>
+      </c>
+      <c r="R5" s="15">
+        <v>0</v>
+      </c>
+      <c r="S5" s="15">
+        <v>0</v>
+      </c>
+      <c r="T5" s="15">
+        <v>0</v>
+      </c>
+      <c r="U5" s="15">
+        <v>0</v>
+      </c>
+      <c r="V5" s="15">
+        <v>0</v>
+      </c>
+      <c r="W5" s="15">
+        <v>0</v>
+      </c>
+      <c r="X5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="17"/>
+      <c r="AQ5" s="17"/>
+      <c r="AR5" s="17"/>
+      <c r="AS5" s="17"/>
+      <c r="AT5" s="17"/>
+      <c r="AU5" s="17"/>
+      <c r="AV5" s="17"/>
+      <c r="AW5" s="17"/>
+      <c r="AX5" s="16"/>
     </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="5"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
-      <c r="AS5" s="9"/>
-      <c r="AT5" s="9"/>
-      <c r="AU5" s="9"/>
-      <c r="AV5" s="9"/>
-      <c r="AW5" s="9"/>
-      <c r="AX5" s="6"/>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AX9" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AP3:AX3"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="AI4:AJ4"/>
     <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AP3:AX3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -1606,12 +1622,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.31527777777777799" right="0.31527777777777799" top="0.31527777777777799" bottom="0.55138888888888904" header="0.511811023622047" footer="0.31527777777777799"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;LOficina Asesora de Tecnologías e Información&amp;CPágina &amp;P de &amp;N&amp;RFecha creación: fecha</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1644,241 +1660,289 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="13"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:44" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="AD2" s="9"/>
+    </row>
+    <row r="3" spans="1:44" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="15" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="AD2" s="1"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="AD3" s="9"/>
+      <c r="AP3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
     </row>
-    <row r="3" spans="1:44" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="17" t="s">
+    <row r="4" spans="1:44" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="AD3" s="1"/>
-      <c r="AP3" s="18" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="18"/>
-      <c r="AR3" s="18"/>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR4" s="13" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR4" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="5"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
+    <row r="5" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
+        <v>0</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0</v>
+      </c>
+      <c r="O5" s="15">
+        <v>0</v>
+      </c>
+      <c r="P5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>0</v>
+      </c>
+      <c r="R5" s="15">
+        <v>0</v>
+      </c>
+      <c r="S5" s="15">
+        <v>0</v>
+      </c>
+      <c r="T5" s="15">
+        <v>0</v>
+      </c>
+      <c r="U5" s="15">
+        <v>0</v>
+      </c>
+      <c r="V5" s="15">
+        <v>0</v>
+      </c>
+      <c r="W5" s="15">
+        <v>0</v>
+      </c>
+      <c r="X5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="17"/>
+      <c r="AQ5" s="17"/>
+      <c r="AR5" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="AG4:AH4"/>
     <mergeCell ref="AI4:AJ4"/>
     <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -1889,12 +1953,12 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.31527777777777799" right="0.31527777777777799" top="0.31527777777777799" bottom="0.55138888888888904" header="0.511811023622047" footer="0.31527777777777799"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;LOficina Asesora de Tecnologías e Información&amp;CPágina &amp;P de &amp;N&amp;RFecha creación: fecha</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1909,7 +1973,7 @@
       <selection pane="bottomRight" activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="59.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="59.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.28515625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -1927,241 +1991,289 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="13"/>
+      <c r="A1" s="8"/>
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:44" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="AD2" s="9"/>
+    </row>
+    <row r="3" spans="1:44" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="15" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="AD2" s="1"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="AD3" s="9"/>
+      <c r="AP3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
     </row>
-    <row r="3" spans="1:44" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="17" t="s">
+    <row r="4" spans="1:44" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="AD3" s="1"/>
-      <c r="AP3" s="18" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="AQ3" s="18"/>
-      <c r="AR3" s="18"/>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="R4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="X4" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC4" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AD4" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH4" s="1"/>
+      <c r="AI4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ4" s="1"/>
+      <c r="AK4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AL4" s="1"/>
+      <c r="AM4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AN4" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="AQ4" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="AR4" s="12" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="4" spans="1:44" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="X4" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z4" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA4" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD4" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG4" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN4" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AO4" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="AP4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AQ4" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR4" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="5"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-      <c r="AG5" s="7"/>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="7"/>
-      <c r="AJ5" s="7"/>
-      <c r="AK5" s="7"/>
-      <c r="AL5" s="7"/>
-      <c r="AM5" s="5"/>
-      <c r="AN5" s="6"/>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="9"/>
-      <c r="AQ5" s="9"/>
-      <c r="AR5" s="9"/>
+    <row r="5" spans="1:44" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="15">
+        <v>0</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0</v>
+      </c>
+      <c r="G5" s="15">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <v>0</v>
+      </c>
+      <c r="I5" s="15">
+        <v>0</v>
+      </c>
+      <c r="J5" s="15">
+        <v>0</v>
+      </c>
+      <c r="K5" s="15">
+        <v>0</v>
+      </c>
+      <c r="L5" s="15">
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
+        <v>0</v>
+      </c>
+      <c r="N5" s="15">
+        <v>0</v>
+      </c>
+      <c r="O5" s="15">
+        <v>0</v>
+      </c>
+      <c r="P5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>0</v>
+      </c>
+      <c r="R5" s="15">
+        <v>0</v>
+      </c>
+      <c r="S5" s="15">
+        <v>0</v>
+      </c>
+      <c r="T5" s="15">
+        <v>0</v>
+      </c>
+      <c r="U5" s="15">
+        <v>0</v>
+      </c>
+      <c r="V5" s="15">
+        <v>0</v>
+      </c>
+      <c r="W5" s="15">
+        <v>0</v>
+      </c>
+      <c r="X5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="14"/>
+      <c r="AE5" s="15">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="15"/>
+      <c r="AK5" s="15"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="16"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="17"/>
+      <c r="AQ5" s="17"/>
+      <c r="AR5" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AI4:AJ4"/>
     <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AP3:AR3"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:G1"/>
@@ -2172,11 +2284,11 @@
     <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.31527777777777799" right="0.31527777777777799" top="0.31527777777777799" bottom="0.55138888888888904" header="0.511811023622047" footer="0.31527777777777799"/>
-  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="5" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddFooter>&amp;LOficina Asesora de Tecnologías e Información&amp;CPágina &amp;P de &amp;N&amp;RFecha creación: fecha</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>